<commit_message>
update with Ilianas comments
</commit_message>
<xml_diff>
--- a/literature_table.xlsx
+++ b/literature_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justincally/Documents/Uni/2018 Semester 1/Sexual Selection/Comparative/Sexual Selection and Speciation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A58ECF-8165-D442-B9CA-4E307EB806BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA7153F-77F4-A34A-813B-B92E9CA1A492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{05F68531-9D15-D44F-9550-7F5ADD0F16ED}"/>
   </bookViews>
@@ -997,7 +997,7 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1243,7 +1243,7 @@
         <v>45</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>44</v>

</xml_diff>